<commit_message>
acertando as questões da relação com o trabalho e o smartbugs no mythril
</commit_message>
<xml_diff>
--- a/mythril/0.24.7_smartbugs-curated/0.24.7_mythril_smartbugs-curated_soma.xlsx
+++ b/mythril/0.24.7_smartbugs-curated/0.24.7_mythril_smartbugs-curated_soma.xlsx
@@ -447,7 +447,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -460,7 +460,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -473,7 +473,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -486,7 +486,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -499,7 +499,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -512,7 +512,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -525,7 +525,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -538,7 +538,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -551,11 +551,11 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Delegatecall to Untrusted Callee</t>
+          <t>Requirement Violation</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -564,11 +564,11 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Requirement Violation</t>
+          <t>Delegatecall to Untrusted Callee</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -577,11 +577,11 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Write to Arbitrary Storage Location</t>
+          <t>Authorization through tx.origin</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -590,7 +590,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -603,11 +603,11 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Authorization through tx.origin</t>
+          <t>Write to Arbitrary Storage Location</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -616,7 +616,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>

</xml_diff>